<commit_message>
Solucion ejercicio 5 fractales
</commit_message>
<xml_diff>
--- a/EjerciciosFractales.xlsx
+++ b/EjerciciosFractales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\Java Intermedio\CursoJatunIntermedioJava\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC2A32C-6619-4465-BA23-D1F207352A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7044042-0E0E-4C75-9EF1-F9C78A28F744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A25993D-CE68-4A63-AC86-6EEAF6634368}"/>
+    <workbookView xWindow="-42000" yWindow="1665" windowWidth="21600" windowHeight="11385" xr2:uid="{1A25993D-CE68-4A63-AC86-6EEAF6634368}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Nivel</t>
   </si>
@@ -79,14 +79,43 @@
   </si>
   <si>
     <t>Diferencia</t>
+  </si>
+  <si>
+    <t>Ejercicio 5</t>
+  </si>
+  <si>
+    <t>f(n-1) +8</t>
+  </si>
+  <si>
+    <t>f(n-1)+ 40</t>
+  </si>
+  <si>
+    <t>f(n-1)+200</t>
+  </si>
+  <si>
+    <t>8*1</t>
+  </si>
+  <si>
+    <t>8*5</t>
+  </si>
+  <si>
+    <t>8*25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -114,9 +143,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -433,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDCBEBC-505D-443C-87BA-A818DFDB59C3}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,28 +475,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -553,6 +583,72 @@
       </c>
       <c r="E7" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>252</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -560,5 +656,6 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="10000" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ejercicio 4 de fractales
</commit_message>
<xml_diff>
--- a/EjerciciosFractales.xlsx
+++ b/EjerciciosFractales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\Java Intermedio\CursoJatunIntermedioJava\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7044042-0E0E-4C75-9EF1-F9C78A28F744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F16999-A1F4-4BC2-B878-79BF67194557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-42000" yWindow="1665" windowWidth="21600" windowHeight="11385" xr2:uid="{1A25993D-CE68-4A63-AC86-6EEAF6634368}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A25993D-CE68-4A63-AC86-6EEAF6634368}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Nivel</t>
   </si>
@@ -100,13 +100,46 @@
   </si>
   <si>
     <t>8*25</t>
+  </si>
+  <si>
+    <t>Ejercicio 4</t>
+  </si>
+  <si>
+    <t>f(n-1) +4</t>
+  </si>
+  <si>
+    <t>f(n-1) + 12</t>
+  </si>
+  <si>
+    <t>f(n-1) + 36</t>
+  </si>
+  <si>
+    <t>f(n-1) + 4 * 1</t>
+  </si>
+  <si>
+    <t>f(n-1) + 4  * 3</t>
+  </si>
+  <si>
+    <t>f(n-1) + 4 * 9</t>
+  </si>
+  <si>
+    <t>f(n-1) + 4 * 3^0</t>
+  </si>
+  <si>
+    <t>f(n-1) + 4 * 3^1</t>
+  </si>
+  <si>
+    <t>f(n-1) + 4 * 3^2</t>
+  </si>
+  <si>
+    <t>f(n-1) + 4 * 3^(n-2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +149,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -143,12 +184,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,15 +505,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDCBEBC-505D-443C-87BA-A818DFDB59C3}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -649,6 +692,84 @@
       </c>
       <c r="D14" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>